<commit_message>
Pricing form and program detail observation and issues fixed.
</commit_message>
<xml_diff>
--- a/WebContent/resources/templates/Pricing_Form_Template.xlsx
+++ b/WebContent/resources/templates/Pricing_Form_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manikandans\Desktop\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manikandans\Desktop\template\27thJuly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
-  <si>
-    <t>Y</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>BEG DATE</t>
   </si>
@@ -53,12 +50,6 @@
     <t>COMMENT</t>
   </si>
   <si>
-    <t>NO CASH DISCOUNT</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>PROD LINE</t>
   </si>
   <si>
@@ -68,40 +59,7 @@
     <t xml:space="preserve"> PART#</t>
   </si>
   <si>
-    <t>60009</t>
-  </si>
-  <si>
-    <t>GUARDEX</t>
-  </si>
-  <si>
-    <t>HPT</t>
-  </si>
-  <si>
-    <t>04817</t>
-  </si>
-  <si>
-    <t>A048</t>
-  </si>
-  <si>
-    <t>60019</t>
-  </si>
-  <si>
-    <t>04807</t>
-  </si>
-  <si>
-    <t>ADD</t>
-  </si>
-  <si>
-    <t>v400</t>
-  </si>
-  <si>
-    <t>hpt</t>
-  </si>
-  <si>
     <t>BUSINESS UNIT</t>
-  </si>
-  <si>
-    <t>CONSUMER</t>
   </si>
 </sst>
 </file>
@@ -467,198 +425,95 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2">
-        <v>42736</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43100</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <v>42736</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43100</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>12.5678</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>42736</v>
-      </c>
-      <c r="C4" s="2">
-        <v>43100</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4">
-        <v>134.47</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>0</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>42736</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43100</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>0</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>42766</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43100</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6">
-        <v>11</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="I6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>